<commit_message>
update: workbook with meeting record
</commit_message>
<xml_diff>
--- a/Documents/Database Design Table.xlsx
+++ b/Documents/Database Design Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuyajing/Documents/Final Year Project/Parsons-problem-generator-solver/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EEA9E3-3C1A-C747-98BB-8E213CB8C36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A543662-8C07-774E-B30C-2EB3D49294A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{50A70F72-41F7-5744-8E19-C4AED27FA47E}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Entity types table" sheetId="1" r:id="rId1"/>
     <sheet name="Relationship types table" sheetId="2" r:id="rId2"/>
     <sheet name="Attributes table" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1477,4 +1478,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40853EF4-D2F8-6D49-8368-6E0359D6820F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add: database creating sql file and automatically generated ER diagram
</commit_message>
<xml_diff>
--- a/Documents/Database Design Table.xlsx
+++ b/Documents/Database Design Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuyajing/Documents/Final Year Project/Parsons-problem-generator-solver/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCB6FF0-BB76-7C49-8B9C-E969F8DD1713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8895B07-C0D5-0943-B95E-A31BA3FBB088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="3" xr2:uid="{50A70F72-41F7-5744-8E19-C4AED27FA47E}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{50A70F72-41F7-5744-8E19-C4AED27FA47E}"/>
   </bookViews>
   <sheets>
     <sheet name="Entity types table" sheetId="1" r:id="rId1"/>
@@ -146,9 +146,6 @@
     <t>Utype</t>
   </si>
   <si>
-    <t>User Type: (admin, teacher, student)</t>
-  </si>
-  <si>
     <t>CID</t>
   </si>
   <si>
@@ -395,10 +392,10 @@
     <t>Promary key: CMTID</t>
   </si>
   <si>
-    <t>Foreign key: UID references User (UID)   ON UPDATE CASCADE ON DELETE SET NULL</t>
-  </si>
-  <si>
-    <t>Foreign key: CID references Class (CID)   ON UPDATE CASCADE ON DELETE SET NULL</t>
+    <t>Foreign key: CID references Class (CID)   ON UPDATE CASCADE ON DELETE NO ACTION</t>
+  </si>
+  <si>
+    <t>Foreign key: UID references User (UID)   ON UPDATE CASCADE ON DELETE NO ACTION</t>
   </si>
   <si>
     <t>Foreign key: UID references User (UID)  ON UPDATE CASCADE ON DELETE NO ACTION</t>
@@ -417,6 +414,9 @@
   </si>
   <si>
     <t>Foreign key: DID references Distractor (DID)  ON UPDATE CASCADE ON DELETE CASCADE</t>
+  </si>
+  <si>
+    <t>User type (admin, teacher, student)</t>
   </si>
 </sst>
 </file>
@@ -814,7 +814,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -825,10 +825,10 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -836,7 +836,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -847,10 +847,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -858,10 +858,10 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -869,10 +869,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -880,32 +880,32 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1029,12 +1029,12 @@
         <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
@@ -1080,7 +1080,7 @@
         <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1109,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95CF970-C72D-834F-A864-FA4089429975}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1194,7 +1194,7 @@
         <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>125</v>
       </c>
       <c r="D6" t="s">
         <v>26</v>
@@ -1202,16 +1202,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D7" t="s">
         <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1219,10 +1219,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
         <v>36</v>
-      </c>
-      <c r="C8" t="s">
-        <v>37</v>
       </c>
       <c r="D8" t="s">
         <v>26</v>
@@ -1233,10 +1233,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
         <v>39</v>
-      </c>
-      <c r="C9" t="s">
-        <v>40</v>
       </c>
       <c r="D9" t="s">
         <v>26</v>
@@ -1247,13 +1247,13 @@
         <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D10" t="s">
         <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1261,10 +1261,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
         <v>42</v>
-      </c>
-      <c r="C11" t="s">
-        <v>43</v>
       </c>
       <c r="D11" t="s">
         <v>26</v>
@@ -1275,21 +1275,21 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
         <v>44</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>45</v>
-      </c>
-      <c r="D12" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
         <v>47</v>
-      </c>
-      <c r="C13" t="s">
-        <v>48</v>
       </c>
       <c r="D13" t="s">
         <v>26</v>
@@ -1300,32 +1300,32 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
         <v>49</v>
-      </c>
-      <c r="D14" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
         <v>51</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
         <v>52</v>
-      </c>
-      <c r="D15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D16" t="s">
         <v>26</v>
@@ -1336,13 +1336,13 @@
         <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D17" t="s">
         <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1350,10 +1350,10 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
         <v>54</v>
-      </c>
-      <c r="C18" t="s">
-        <v>55</v>
       </c>
       <c r="D18" t="s">
         <v>26</v>
@@ -1364,38 +1364,38 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D20" t="s">
         <v>26</v>
       </c>
       <c r="E20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D21" t="s">
         <v>26</v>
@@ -1406,16 +1406,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D22" t="s">
         <v>26</v>
       </c>
       <c r="E22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1423,10 +1423,10 @@
         <v>10</v>
       </c>
       <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
         <v>56</v>
-      </c>
-      <c r="C23" t="s">
-        <v>57</v>
       </c>
       <c r="D23" t="s">
         <v>26</v>
@@ -1437,27 +1437,27 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D25" t="s">
         <v>26</v>
       </c>
       <c r="E25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1465,10 +1465,10 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
         <v>59</v>
-      </c>
-      <c r="C26" t="s">
-        <v>60</v>
       </c>
       <c r="D26" t="s">
         <v>26</v>
@@ -1479,27 +1479,27 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D28" t="s">
         <v>26</v>
       </c>
       <c r="E28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1507,10 +1507,10 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
         <v>61</v>
-      </c>
-      <c r="C29" t="s">
-        <v>62</v>
       </c>
       <c r="D29" t="s">
         <v>26</v>
@@ -1521,38 +1521,38 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
         <v>63</v>
       </c>
-      <c r="C30" t="s">
-        <v>64</v>
-      </c>
       <c r="D30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D31" t="s">
         <v>26</v>
       </c>
       <c r="E31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" t="s">
         <v>87</v>
-      </c>
-      <c r="C32" t="s">
-        <v>88</v>
       </c>
       <c r="D32" t="s">
         <v>26</v>
@@ -1563,27 +1563,27 @@
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D34" t="s">
         <v>26</v>
       </c>
       <c r="E34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1595,15 +1595,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40853EF4-D2F8-6D49-8368-6E0359D6820F}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:G31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1626,7 +1626,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1646,7 +1646,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1657,7 +1657,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1688,7 +1688,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1699,7 +1699,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1710,7 +1710,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1730,7 +1730,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1741,7 +1741,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1752,7 +1752,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1772,7 +1772,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1783,7 +1783,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1794,7 +1794,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1814,7 +1814,7 @@
     </row>
     <row r="21" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1825,7 +1825,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1836,7 +1836,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1856,7 +1856,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1878,7 +1878,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1898,7 +1898,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1909,7 +1909,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1920,7 +1920,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1940,7 +1940,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1951,7 +1951,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1962,7 +1962,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>

</xml_diff>

<commit_message>
update: workbook(Progree report) and database design
</commit_message>
<xml_diff>
--- a/Documents/Database Design Table.xlsx
+++ b/Documents/Database Design Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuyajing/Documents/Final Year Project/Parsons-problem-generator-solver/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD56EDE2-E110-264F-9F3E-2C28B5D9808F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1E0AF7-8421-6B45-8E0D-B61E87A491C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{50A70F72-41F7-5744-8E19-C4AED27FA47E}"/>
+    <workbookView xWindow="-20" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{50A70F72-41F7-5744-8E19-C4AED27FA47E}"/>
   </bookViews>
   <sheets>
     <sheet name="Entity types table" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="138">
   <si>
     <t>Entry name</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Fragment</t>
   </si>
   <si>
-    <t xml:space="preserve">Each question is set up by a teacher. Each question can have several solutions.   </t>
-  </si>
-  <si>
     <t>Entity name</t>
   </si>
   <si>
@@ -194,9 +191,6 @@
     <t>PIC</t>
   </si>
   <si>
-    <t>Question picture name</t>
-  </si>
-  <si>
     <t>Null allowed</t>
   </si>
   <si>
@@ -239,9 +233,6 @@
     <t>Block</t>
   </si>
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
     <t>A general term describing the class</t>
   </si>
   <si>
@@ -266,27 +257,9 @@
     <t>A general term describing the block of a specific solution containing one or multiple code fragment(s)</t>
   </si>
   <si>
-    <t>A general term describing the comment related to a specific code fragment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Each fragment belongs to one solution. Each fragment can have a corresponding distractor or comment. </t>
-  </si>
-  <si>
-    <t>Each block belongs to one solution. Each block contains one or multiple code fragment(s).</t>
-  </si>
-  <si>
-    <t>Each code fragment may have a related comment.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Each teacher has a number of classes. Each student belongs to one class. Each teacher can input a number of questions. </t>
   </si>
   <si>
-    <t>Each distractor has a corresponding prepared feedback.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Each solution belongs to one block. Each solution has a group of blocks. </t>
-  </si>
-  <si>
     <t>Each distractor has a related fragment.</t>
   </si>
   <si>
@@ -299,18 +272,6 @@
     <t>BID</t>
   </si>
   <si>
-    <t>CMTID</t>
-  </si>
-  <si>
-    <t>Uniquely identifies a comment</t>
-  </si>
-  <si>
-    <t>Comment content</t>
-  </si>
-  <si>
-    <t>Question tag (standard, multiple solutions, insert key code )</t>
-  </si>
-  <si>
     <t>Uniquely identifies a block</t>
   </si>
   <si>
@@ -350,9 +311,6 @@
     <t>References Distractor (DID)</t>
   </si>
   <si>
-    <t>Question (QID, Date, Scope, Description, PIC, Tag, UID)</t>
-  </si>
-  <si>
     <t>Primary key: QID</t>
   </si>
   <si>
@@ -362,15 +320,9 @@
     <t>Primary key: SID</t>
   </si>
   <si>
-    <t>Block (BID, SID)</t>
-  </si>
-  <si>
     <t>Primary key: BID</t>
   </si>
   <si>
-    <t>Fragment (FID, Code, BID)</t>
-  </si>
-  <si>
     <t>Primary key: FID</t>
   </si>
   <si>
@@ -386,12 +338,6 @@
     <t>Primary key: FBID</t>
   </si>
   <si>
-    <t>Comment (CMTID, Content, FID)</t>
-  </si>
-  <si>
-    <t>Promary key: CMTID</t>
-  </si>
-  <si>
     <t>Foreign key: CID references Class (CID)   ON UPDATE CASCADE ON DELETE NO ACTION</t>
   </si>
   <si>
@@ -404,9 +350,6 @@
     <t>Foreign key: QID references Question (QID)  ON UPDATE CASCADE ON DELETE CASCADE</t>
   </si>
   <si>
-    <t>Foreign key: SID references Solution (SID)  ON UPDATE CASCADE ON DELETE CASCADE</t>
-  </si>
-  <si>
     <t>Foreign key: BID references Block (BID)  ON UPDATE CASCADE ON DELETE CASCADE</t>
   </si>
   <si>
@@ -417,6 +360,99 @@
   </si>
   <si>
     <t>User type (admin, teacher, student)</t>
+  </si>
+  <si>
+    <t>Fragment tag (context, comment)</t>
+  </si>
+  <si>
+    <t>A general term describing the difficulty level</t>
+  </si>
+  <si>
+    <t>Fragment (FID, Code, Tag, BID)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each question is set up by a teacher. Each question can have oen or multiple solutions.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each solution belongs to one question. Each solution has one or multiple difficulty levels. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each fragment belongs to one block. Each fragment can have a corresponding distractor. </t>
+  </si>
+  <si>
+    <t>Each distractor has a corresponding predefined feedback.</t>
+  </si>
+  <si>
+    <t>Each block is related with a difficulty level. Each block contains one or multiple code fragment(s).</t>
+  </si>
+  <si>
+    <t>Each difficulty level points to a number of blocks. Each difficulty level belongs to a solution</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>DifficultyLevel</t>
+  </si>
+  <si>
+    <t>DLID</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>BlockSeq</t>
+  </si>
+  <si>
+    <t>Uniquely identifies a difficulty level</t>
+  </si>
+  <si>
+    <t>Describes the level</t>
+  </si>
+  <si>
+    <t>Sequence of containing block</t>
+  </si>
+  <si>
+    <t>References DifficultyLevel (DLID)</t>
+  </si>
+  <si>
+    <t>Foreign key: DLID references DifficultyLevel (DLID)  ON UPDATE CASCADE ON DELETE CASCADE</t>
+  </si>
+  <si>
+    <t>DifficultyLevel (DLID, Level, BlockSeq, SID)</t>
+  </si>
+  <si>
+    <t>Primary key: DLID</t>
+  </si>
+  <si>
+    <t>Foreign key: SID references Solution (SID) ON UPDATE CASCADE ON DELETE CASCADE</t>
+  </si>
+  <si>
+    <t>SolutionSeq</t>
+  </si>
+  <si>
+    <t>Sequence of subsolution</t>
+  </si>
+  <si>
+    <t>Question picture name(s)</t>
+  </si>
+  <si>
+    <t>Question (QID, Date, Scope, Description, PIC, Tag, SolutionSeq, UID)</t>
+  </si>
+  <si>
+    <t>FragmentSeq</t>
+  </si>
+  <si>
+    <t>Sequence of fragments</t>
+  </si>
+  <si>
+    <t>Block tag (single fragment, multiple fragments)</t>
+  </si>
+  <si>
+    <t>Question tag (standard, multiple solutions, insert key code, multiple steps )</t>
+  </si>
+  <si>
+    <t>Block (BID, Tag, FragmentSeq, DLID)</t>
   </si>
 </sst>
 </file>
@@ -457,12 +493,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -783,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795E7953-B284-B643-BA1D-306296F400FF}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="113" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -814,7 +850,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -822,13 +858,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -836,10 +872,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -847,10 +883,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -858,10 +894,10 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -869,10 +905,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -880,32 +916,32 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D9" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>117</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>108</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -918,7 +954,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -932,16 +968,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -952,30 +988,30 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -983,16 +1019,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -1003,13 +1039,13 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
@@ -1020,30 +1056,30 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1054,13 +1090,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
         <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
@@ -1068,36 +1104,36 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
       <c r="E9" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>117</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1107,111 +1143,111 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95CF970-C72D-834F-A864-FA4089429975}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
-    <col min="3" max="3" width="55.5" customWidth="1"/>
+    <col min="3" max="3" width="66.33203125" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
       <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
         <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
         <v>29</v>
       </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1219,41 +1255,41 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
         <v>35</v>
       </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
       <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
         <v>26</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" t="s">
-        <v>39</v>
-      </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1261,38 +1297,38 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
         <v>41</v>
       </c>
-      <c r="C11" t="s">
-        <v>42</v>
-      </c>
       <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
         <v>26</v>
-      </c>
-      <c r="E11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
         <v>43</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>44</v>
-      </c>
-      <c r="D12" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
         <v>46</v>
       </c>
-      <c r="C13" t="s">
-        <v>47</v>
-      </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1300,290 +1336,351 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
         <v>48</v>
-      </c>
-      <c r="D14" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" t="s">
         <v>50</v>
-      </c>
-      <c r="C15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
       <c r="C17" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
       <c r="D17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
         <v>26</v>
-      </c>
-      <c r="E17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="D20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" t="s">
         <v>26</v>
       </c>
-      <c r="E20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" t="s">
-        <v>90</v>
-      </c>
-      <c r="D21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" t="s">
-        <v>99</v>
-      </c>
-      <c r="D22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>10</v>
-      </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" t="s">
-        <v>27</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>57</v>
+        <v>133</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>134</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>25</v>
+      </c>
+      <c r="E24" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="C25" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="D25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" t="s">
         <v>26</v>
-      </c>
-      <c r="E26" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="C28" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" t="s">
         <v>26</v>
-      </c>
-      <c r="E28" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" t="s">
+        <v>88</v>
+      </c>
+      <c r="D32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
         <v>58</v>
       </c>
-      <c r="C31" t="s">
-        <v>102</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" t="s">
         <v>26</v>
       </c>
-      <c r="E31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" t="s">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" t="s">
         <v>86</v>
       </c>
-      <c r="C32" t="s">
-        <v>87</v>
-      </c>
-      <c r="D32" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" t="s">
-        <v>101</v>
-      </c>
-      <c r="D34" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" t="s">
-        <v>37</v>
+      <c r="D39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1596,212 +1693,215 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A18" sqref="A18:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="30.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="A19" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
@@ -1813,37 +1913,37 @@
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="A22" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="A23" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
@@ -1855,37 +1955,37 @@
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="A25" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="A26" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="A27" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
@@ -1897,37 +1997,37 @@
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="A29" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+      <c r="A30" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
+      <c r="A31" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
@@ -1939,50 +2039,53 @@
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
+      <c r="A33" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="A34" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
+      <c r="A35" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A31:G31"/>
     <mergeCell ref="A33:G33"/>
     <mergeCell ref="A34:G34"/>
     <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A11:G11"/>
     <mergeCell ref="A29:G29"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="A15:G15"/>
@@ -1990,16 +2093,13 @@
     <mergeCell ref="A18:G18"/>
     <mergeCell ref="A19:G19"/>
     <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A31:G31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update: database.py, change the 'type' attributes in question, solution, block, fragment
</commit_message>
<xml_diff>
--- a/Documents/Database Design Table.xlsx
+++ b/Documents/Database Design Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuyajing/Documents/Final Year Project/Parsons-problem-generator-solver/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62483E2-DE36-204E-A331-F4B83D208894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF93126-2428-5A40-ABC5-069D0102B1E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="2" xr2:uid="{50A70F72-41F7-5744-8E19-C4AED27FA47E}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="141">
   <si>
     <t>Entry name</t>
   </si>
@@ -263,9 +263,6 @@
     <t>Each distractor has a related fragment.</t>
   </si>
   <si>
-    <t>Tag</t>
-  </si>
-  <si>
     <t>Solution file name</t>
   </si>
   <si>
@@ -314,9 +311,6 @@
     <t>Primary key: QID</t>
   </si>
   <si>
-    <t>Solution (SID, Sname, QID)</t>
-  </si>
-  <si>
     <t>Primary key: SID</t>
   </si>
   <si>
@@ -362,15 +356,6 @@
     <t>User type (admin, teacher, student)</t>
   </si>
   <si>
-    <t>Fragment tag (context, comment)</t>
-  </si>
-  <si>
-    <t>A general term describing the difficulty level</t>
-  </si>
-  <si>
-    <t>Fragment (FID, Code, Tag, BID)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Each question is set up by a teacher. Each question can have oen or multiple solutions.   </t>
   </si>
   <si>
@@ -431,35 +416,157 @@
     <t>Question picture name(s)</t>
   </si>
   <si>
-    <t>Question (QID, Date, Scope, Description, PIC, Tag, SolutionSeq, UID)</t>
-  </si>
-  <si>
     <t>FragmentSeq</t>
   </si>
   <si>
     <t>Sequence of fragments</t>
   </si>
   <si>
-    <t>Block tag (single fragment, multiple fragments)</t>
-  </si>
-  <si>
-    <t>Question tag (standard, multiple solutions, insert key code, multiple steps )</t>
-  </si>
-  <si>
-    <t>Block (BID, Tag, FragmentSeq, DLID)</t>
-  </si>
-  <si>
     <t>Sequence of containing block (s)</t>
   </si>
   <si>
     <t>Sequence of subsolutions</t>
+  </si>
+  <si>
+    <t>Question Name</t>
+  </si>
+  <si>
+    <t>QName</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Block types (single fragment, multiple fragments (context), multiple fragments (unit))</t>
+  </si>
+  <si>
+    <r>
+      <t>Solution (SID, Sname,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> Type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, QID)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Block (BID, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, FragmentSeq, DLID)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fragment (FID, Code, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, BID)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Question (QID, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>QName</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Date, Scope, Description, PIC, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, SolutionSeq, UID)</t>
+    </r>
+  </si>
+  <si>
+    <t>A copy of the original solutions. It is used to record different ways of organizing blocks in different difficulty levels</t>
+  </si>
+  <si>
+    <t>Question types (singe solution, multiple solutions, multi-step solutions )</t>
+  </si>
+  <si>
+    <t>Solution types (fixed order, not fixed order)</t>
+  </si>
+  <si>
+    <t>Fragment types (code, comment)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -467,13 +574,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -493,16 +611,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -820,13 +938,13 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView zoomScale="113" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B16" sqref="B16:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="90.6640625" customWidth="1"/>
+    <col min="2" max="2" width="99.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.5" customWidth="1"/>
     <col min="4" max="4" width="65.6640625" customWidth="1"/>
   </cols>
@@ -875,7 +993,7 @@
         <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -886,7 +1004,7 @@
         <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -897,7 +1015,7 @@
         <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -919,7 +1037,7 @@
         <v>70</v>
       </c>
       <c r="D8" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -930,18 +1048,18 @@
         <v>71</v>
       </c>
       <c r="D9" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B10" t="s">
-        <v>108</v>
+        <v>112</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="D10" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1065,7 +1183,7 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1121,13 +1239,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
@@ -1143,17 +1261,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95CF970-C72D-834F-A864-FA4089429975}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
-    <col min="3" max="3" width="66.33203125" customWidth="1"/>
+    <col min="3" max="3" width="87.6640625" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
@@ -1230,7 +1348,7 @@
         <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
         <v>25</v>
@@ -1241,7 +1359,7 @@
         <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7" t="s">
         <v>25</v>
@@ -1283,7 +1401,7 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
@@ -1309,380 +1427,399 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" t="s">
-        <v>44</v>
+    <row r="12" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>129</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
         <v>48</v>
       </c>
-      <c r="E15" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>128</v>
-      </c>
-      <c r="C17" t="s">
-        <v>137</v>
-      </c>
-      <c r="D17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>23</v>
       </c>
-      <c r="C18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="C19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>4</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>51</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>52</v>
       </c>
-      <c r="D19" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" t="s">
-        <v>26</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>133</v>
+        <v>84</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
       </c>
+      <c r="E23" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>63</v>
+      </c>
       <c r="B24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D24" t="s">
-        <v>25</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="D25" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" t="s">
+        <v>126</v>
+      </c>
+      <c r="D26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>118</v>
-      </c>
-      <c r="C25" t="s">
-        <v>123</v>
-      </c>
-      <c r="D25" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" t="s">
-        <v>25</v>
-      </c>
-      <c r="E26" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>55</v>
+        <v>113</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>118</v>
       </c>
       <c r="D27" t="s">
-        <v>48</v>
+        <v>25</v>
+      </c>
+      <c r="E27" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="D28" t="s">
         <v>25</v>
       </c>
       <c r="E28" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="D29" t="s">
-        <v>25</v>
-      </c>
-      <c r="E29" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" t="s">
-        <v>25</v>
-      </c>
-      <c r="E30" t="s">
-        <v>26</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
         <v>55</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C33" t="s">
         <v>55</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D33" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" t="s">
-        <v>88</v>
-      </c>
-      <c r="D32" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" t="s">
-        <v>59</v>
-      </c>
-      <c r="D33" t="s">
-        <v>25</v>
-      </c>
-      <c r="E33" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
         <v>60</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C36" t="s">
         <v>61</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D36" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" t="s">
-        <v>89</v>
-      </c>
-      <c r="D35" t="s">
-        <v>25</v>
-      </c>
-      <c r="E35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>117</v>
-      </c>
-      <c r="B36" t="s">
-        <v>118</v>
-      </c>
-      <c r="C36" t="s">
-        <v>121</v>
-      </c>
-      <c r="D36" t="s">
-        <v>25</v>
-      </c>
-      <c r="E36" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>119</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="D37" t="s">
         <v>25</v>
       </c>
+      <c r="E37" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>112</v>
+      </c>
       <c r="B38" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C38" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="D38" t="s">
-        <v>48</v>
+        <v>25</v>
+      </c>
+      <c r="E38" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
         <v>51</v>
       </c>
-      <c r="C39" t="s">
-        <v>86</v>
-      </c>
-      <c r="D39" t="s">
-        <v>25</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="C41" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1693,10 +1830,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40853EF4-D2F8-6D49-8368-6E0359D6820F}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:G18"/>
+      <selection activeCell="A9" sqref="A9:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1704,9 +1841,9 @@
     <col min="7" max="7" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1714,11 +1851,10 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1727,9 +1863,9 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1738,18 +1874,18 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1758,9 +1894,9 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1769,9 +1905,9 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1780,18 +1916,18 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1800,9 +1936,9 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1811,9 +1947,9 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1822,18 +1958,18 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>91</v>
+        <v>133</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1842,9 +1978,9 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1853,9 +1989,9 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1864,18 +2000,18 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1886,7 +2022,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1896,15 +2032,15 @@
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="A19" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
@@ -1916,37 +2052,37 @@
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="A21" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+      <c r="A22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="A23" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
@@ -1958,37 +2094,37 @@
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+      <c r="A25" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="A26" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
+      <c r="A27" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
@@ -2000,37 +2136,37 @@
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+      <c r="A29" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
+      <c r="A30" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
+      <c r="A31" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
@@ -2043,7 +2179,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2054,7 +2190,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -2065,7 +2201,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -2076,17 +2212,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A22:G22"/>
     <mergeCell ref="A33:G33"/>
     <mergeCell ref="A34:G34"/>
     <mergeCell ref="A35:G35"/>
@@ -2103,6 +2228,17 @@
     <mergeCell ref="A29:G29"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A30:G30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix bugs, build basic original codes showing page
</commit_message>
<xml_diff>
--- a/Documents/Database Design Table.xlsx
+++ b/Documents/Database Design Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuyajing/Documents/Final Year Project/Parsons-problem-generator-solver/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF93126-2428-5A40-ABC5-069D0102B1E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318B34E1-ABD5-9A47-A704-8C2A7080B3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="2" xr2:uid="{50A70F72-41F7-5744-8E19-C4AED27FA47E}"/>
   </bookViews>
@@ -428,16 +428,13 @@
     <t>Sequence of subsolutions</t>
   </si>
   <si>
+    <t>Qname</t>
+  </si>
+  <si>
     <t>Question Name</t>
   </si>
   <si>
-    <t>QName</t>
-  </si>
-  <si>
     <t>Type</t>
-  </si>
-  <si>
-    <t>Block types (single fragment, multiple fragments (context), multiple fragments (unit))</t>
   </si>
   <si>
     <r>
@@ -556,17 +553,50 @@
     <t>Question types (singe solution, multiple solutions, multi-step solutions )</t>
   </si>
   <si>
-    <t>Solution types (fixed order, not fixed order)</t>
-  </si>
-  <si>
     <t>Fragment types (code, comment)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Solution types (fixed order, not fixed order, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>insert key code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Block types (single fragment, multiple fragments (context), multiple fragments (unit), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>multiple fragments (standard))</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -577,6 +607,11 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
@@ -1056,7 +1091,7 @@
         <v>112</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D10" t="s">
         <v>110</v>
@@ -1264,14 +1299,14 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
-    <col min="3" max="3" width="87.6640625" customWidth="1"/>
+    <col min="3" max="3" width="120.1640625" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
@@ -1429,10 +1464,10 @@
     </row>
     <row r="12" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>130</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>129</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>25</v>
@@ -1490,7 +1525,7 @@
         <v>131</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>25</v>
@@ -1596,7 +1631,7 @@
         <v>131</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>25</v>
@@ -1663,7 +1698,7 @@
         <v>131</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>25</v>
@@ -1927,7 +1962,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1969,7 +2004,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2011,7 +2046,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -2053,7 +2088,7 @@
     </row>
     <row r="21" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>

</xml_diff>

<commit_message>
redesign the input question process and add new webpage to enter question type
</commit_message>
<xml_diff>
--- a/Documents/Database Design Table.xlsx
+++ b/Documents/Database Design Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuyajing/Documents/Final Year Project/Parsons-problem-generator-solver/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C91918-E9F4-4245-BBDF-33338B478BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885233D6-1963-7E40-89E5-D34C5B349168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="2" xr2:uid="{50A70F72-41F7-5744-8E19-C4AED27FA47E}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Attributes table" sheetId="3" r:id="rId3"/>
     <sheet name="Logical data model" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="132">
   <si>
     <t>Entry name</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Distractor</t>
   </si>
   <si>
-    <t>Feedback</t>
-  </si>
-  <si>
     <t>Class</t>
   </si>
   <si>
@@ -215,18 +212,6 @@
     <t>Uniquely identifies a distractor</t>
   </si>
   <si>
-    <t>FBID</t>
-  </si>
-  <si>
-    <t>Uniquely identifies a feedback</t>
-  </si>
-  <si>
-    <t>Content</t>
-  </si>
-  <si>
-    <t>Feedback content</t>
-  </si>
-  <si>
     <t>Sname</t>
   </si>
   <si>
@@ -251,9 +236,6 @@
     <t>A general term describing the distractor of a specific code fragment</t>
   </si>
   <si>
-    <t>A general term describing the feedback related to a specific distractor</t>
-  </si>
-  <si>
     <t>A general term describing the block of a specific solution containing one or multiple code fragment(s)</t>
   </si>
   <si>
@@ -305,9 +287,6 @@
     <t>References Fragment (FID)</t>
   </si>
   <si>
-    <t>References Distractor (DID)</t>
-  </si>
-  <si>
     <t>Primary key: QID</t>
   </si>
   <si>
@@ -326,12 +305,6 @@
     <t>Primary key: DID</t>
   </si>
   <si>
-    <t>Feedback (FBID, Content, DID)</t>
-  </si>
-  <si>
-    <t>Primary key: FBID</t>
-  </si>
-  <si>
     <t>Foreign key: CID references Class (CID)   ON UPDATE CASCADE ON DELETE NO ACTION</t>
   </si>
   <si>
@@ -350,9 +323,6 @@
     <t>Foreign key: FID references Fragment (FID)  ON UPDATE CASCADE ON DELETE CASCADE</t>
   </si>
   <si>
-    <t>Foreign key: DID references Distractor (DID)  ON UPDATE CASCADE ON DELETE CASCADE</t>
-  </si>
-  <si>
     <t>User type (admin, teacher, student)</t>
   </si>
   <si>
@@ -363,9 +333,6 @@
   </si>
   <si>
     <t xml:space="preserve">Each fragment belongs to one block. Each fragment can have a corresponding distractor. </t>
-  </si>
-  <si>
-    <t>Each distractor has a corresponding predefined feedback.</t>
   </si>
   <si>
     <t>Each block is related with a difficulty level. Each block contains one or multiple code fragment(s).</t>
@@ -550,37 +517,17 @@
     <t>A copy of the original solutions. It is used to record different ways of organizing blocks in different difficulty levels</t>
   </si>
   <si>
-    <t>Question types (singe solution, multiple solutions, multi-step solutions )</t>
-  </si>
-  <si>
-    <t>Fragment types (code, comment)</t>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Reason to set this distractor</t>
+  </si>
+  <si>
+    <t>Solution types (reference, not reference)</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Solution types (fixed order, not fixed order, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>insert key code</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Block types (single fragment, multiple fragments (context), multiple fragments (unit), </t>
+      <t>Block types (combine, not combine</t>
     </r>
     <r>
       <rPr>
@@ -588,8 +535,14 @@
         <color theme="1"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>multiple fragments (standard))</t>
+      <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>Fragment types (context, not context, key code, not key code, comment, code)</t>
+  </si>
+  <si>
+    <t>Question types (traditional, context, insert key code, check only inside block, multiple steps, compare data structure implementation, compare algorithm, link together, algorithm analysis )</t>
   </si>
 </sst>
 </file>
@@ -649,13 +602,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -970,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795E7953-B284-B643-BA1D-306296F400FF}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="113" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B17"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1000,24 +953,24 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1025,10 +978,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1036,21 +989,21 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1058,43 +1011,32 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" t="s">
-        <v>71</v>
+        <v>101</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="D9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>112</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D10" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1104,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{260A0A7F-1E09-E642-8F7D-33314A897E2B}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1121,16 +1063,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -1138,50 +1080,50 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -1192,13 +1134,13 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
@@ -1209,47 +1151,47 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
       <c r="E6" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
         <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
@@ -1257,36 +1199,19 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>101</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>112</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1296,153 +1221,153 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95CF970-C72D-834F-A864-FA4089429975}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
-    <col min="3" max="3" width="120.1640625" customWidth="1"/>
+    <col min="3" max="3" width="163.33203125" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
       <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
         <v>25</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
         <v>34</v>
       </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
       <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
         <v>25</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
         <v>37</v>
       </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1450,49 +1375,49 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
         <v>40</v>
       </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
       <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
         <v>25</v>
       </c>
-      <c r="E11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>25</v>
+    </row>
+    <row r="12" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
         <v>42</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>43</v>
-      </c>
-      <c r="D13" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
         <v>45</v>
       </c>
-      <c r="C14" t="s">
-        <v>46</v>
-      </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1500,63 +1425,66 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
         <v>47</v>
-      </c>
-      <c r="D15" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
         <v>49</v>
       </c>
-      <c r="C16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D16" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="5" t="s">
+    </row>
+    <row r="17" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>25</v>
+      <c r="D17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C18" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1564,161 +1492,170 @@
         <v>4</v>
       </c>
       <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
         <v>51</v>
       </c>
-      <c r="C20" t="s">
-        <v>52</v>
-      </c>
       <c r="D20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" t="s">
         <v>25</v>
-      </c>
-      <c r="E20" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>139</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" t="s">
         <v>25</v>
       </c>
-      <c r="E24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>25</v>
+    </row>
+    <row r="25" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C26" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D26" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C27" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="D27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
         <v>53</v>
       </c>
-      <c r="C28" t="s">
-        <v>54</v>
-      </c>
       <c r="D28" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" t="s">
         <v>25</v>
-      </c>
-      <c r="E28" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D29" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C31" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1726,136 +1663,105 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" t="s">
         <v>56</v>
       </c>
-      <c r="C32" t="s">
-        <v>57</v>
-      </c>
       <c r="D32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" t="s">
         <v>25</v>
-      </c>
-      <c r="E32" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>53</v>
+        <v>126</v>
       </c>
       <c r="C34" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="D34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" t="s">
         <v>25</v>
-      </c>
-      <c r="E34" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" t="s">
-        <v>25</v>
-      </c>
-      <c r="E35" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
-        <v>60</v>
-      </c>
-      <c r="C36" t="s">
-        <v>61</v>
-      </c>
-      <c r="D36" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>56</v>
+        <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="D37" t="s">
-        <v>25</v>
-      </c>
-      <c r="E37" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>112</v>
-      </c>
       <c r="B38" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C38" t="s">
         <v>116</v>
       </c>
       <c r="D38" t="s">
-        <v>25</v>
-      </c>
-      <c r="E38" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>114</v>
+        <v>50</v>
       </c>
       <c r="C39" t="s">
-        <v>117</v>
+        <v>79</v>
       </c>
       <c r="D39" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
-        <v>115</v>
-      </c>
-      <c r="C40" t="s">
-        <v>127</v>
-      </c>
-      <c r="D40" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>51</v>
-      </c>
-      <c r="C41" t="s">
-        <v>85</v>
-      </c>
-      <c r="D41" t="s">
-        <v>25</v>
-      </c>
-      <c r="E41" t="s">
-        <v>36</v>
+        <v>24</v>
+      </c>
+      <c r="E39" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1865,10 +1771,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40853EF4-D2F8-6D49-8368-6E0359D6820F}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:G9"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1878,7 +1784,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1889,7 +1795,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1900,7 +1806,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1920,7 +1826,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1931,7 +1837,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1942,7 +1848,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1962,7 +1868,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1973,7 +1879,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1984,7 +1890,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2004,7 +1910,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2015,7 +1921,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2026,7 +1932,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -2046,7 +1952,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -2057,7 +1963,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -2067,15 +1973,15 @@
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="A19" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
@@ -2087,37 +1993,37 @@
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="A21" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
@@ -2129,37 +2035,37 @@
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
@@ -2171,85 +2077,52 @@
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="A29" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+      <c r="A30" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
+      <c r="A31" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="A35:G35"/>
+  <mergeCells count="24">
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A31:G31"/>
     <mergeCell ref="A13:G13"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
@@ -2260,20 +2133,8 @@
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="A10:G10"/>
     <mergeCell ref="A11:G11"/>
-    <mergeCell ref="A29:G29"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="A15:G15"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="A30:G30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add function about inserting key code (set this type, mark key code, show key code)
</commit_message>
<xml_diff>
--- a/Documents/Database Design Table.xlsx
+++ b/Documents/Database Design Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuyajing/Documents/Final Year Project/Parsons-problem-generator-solver/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885233D6-1963-7E40-89E5-D34C5B349168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965C3738-76A9-7546-ABB8-E39180423894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="2" xr2:uid="{50A70F72-41F7-5744-8E19-C4AED27FA47E}"/>
   </bookViews>
@@ -542,7 +542,7 @@
     <t>Fragment types (context, not context, key code, not key code, comment, code)</t>
   </si>
   <si>
-    <t>Question types (traditional, context, insert key code, check only inside block, multiple steps, compare data structure implementation, compare algorithm, link together, algorithm analysis )</t>
+    <t>Question types (traditional, context, insert-key-code, check-only-inside-block, multiple-steps, compare-data-structure-implementation, compare-algorithm, link-together, algorithm-analysis )</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1049,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1190,8 +1190,8 @@
       <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
-        <v>14</v>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
add different difficulty level
</commit_message>
<xml_diff>
--- a/Documents/Database Design Table.xlsx
+++ b/Documents/Database Design Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuyajing/Documents/Final Year Project/Parsons-problem-generator-solver/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965C3738-76A9-7546-ABB8-E39180423894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8068DECA-1B8D-F44E-81B3-52C0CFE8F83F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="2" xr2:uid="{50A70F72-41F7-5744-8E19-C4AED27FA47E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="3" xr2:uid="{50A70F72-41F7-5744-8E19-C4AED27FA47E}"/>
   </bookViews>
   <sheets>
     <sheet name="Entity types table" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="141">
   <si>
     <t>Entry name</t>
   </si>
@@ -514,9 +514,6 @@
     </r>
   </si>
   <si>
-    <t>A copy of the original solutions. It is used to record different ways of organizing blocks in different difficulty levels</t>
-  </si>
-  <si>
     <t>Reason</t>
   </si>
   <si>
@@ -543,6 +540,36 @@
   </si>
   <si>
     <t>Question types (traditional, context, insert-key-code, check-only-inside-block, multiple-steps, compare-data-structure-implementation, compare-algorithm, link-together, algorithm-analysis )</t>
+  </si>
+  <si>
+    <t>EasierVersionPointer</t>
+  </si>
+  <si>
+    <t>A copy of the original solutions. It is used to record different ways of organizing blocks in different difficulty levels (Legacy)</t>
+  </si>
+  <si>
+    <t>If a question can get a easier version by setting as other types of question with more hints (like 'context', 'insert key code'), ids of origianl question and easier one will be recorded here.</t>
+  </si>
+  <si>
+    <t>Each question can have a eaiser question.</t>
+  </si>
+  <si>
+    <t>OriginalQID</t>
+  </si>
+  <si>
+    <t>EasierVersionQID</t>
+  </si>
+  <si>
+    <t>Original Question ID</t>
+  </si>
+  <si>
+    <t>Easier Version QID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EasierVersionPointer(OriginalQID, EasierVersionQID) </t>
+  </si>
+  <si>
+    <t>PrimaryKey: OriginalQID</t>
   </si>
 </sst>
 </file>
@@ -594,7 +621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -604,9 +631,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -923,16 +953,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795E7953-B284-B643-BA1D-306296F400FF}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView zoomScale="113" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="99.6640625" customWidth="1"/>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="162.1640625" customWidth="1"/>
     <col min="3" max="3" width="15.5" customWidth="1"/>
     <col min="4" max="4" width="65.6640625" customWidth="1"/>
   </cols>
@@ -1033,10 +1063,21 @@
         <v>101</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="D9" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1221,10 +1262,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95CF970-C72D-834F-A864-FA4089429975}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView zoomScale="86" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1450,7 +1491,7 @@
         <v>120</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>24</v>
@@ -1520,7 +1561,7 @@
         <v>120</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>24</v>
@@ -1565,7 +1606,7 @@
         <v>120</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>24</v>
@@ -1635,7 +1676,7 @@
         <v>120</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>24</v>
@@ -1688,10 +1729,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" t="s">
         <v>126</v>
-      </c>
-      <c r="C34" t="s">
-        <v>127</v>
       </c>
       <c r="D34" t="s">
         <v>47</v>
@@ -1762,6 +1803,34 @@
       </c>
       <c r="E39" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1771,10 +1840,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40853EF4-D2F8-6D49-8368-6E0359D6820F}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1783,37 +1852,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
@@ -1825,37 +1894,37 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
@@ -1867,37 +1936,37 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
@@ -1909,37 +1978,37 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
@@ -1951,37 +2020,37 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
@@ -1993,37 +2062,37 @@
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
@@ -2035,37 +2104,37 @@
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
@@ -2077,49 +2146,64 @@
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="33" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+    </row>
+    <row r="34" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A22:G22"/>
+  <mergeCells count="26">
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A34:G34"/>
     <mergeCell ref="A29:G29"/>
     <mergeCell ref="A30:G30"/>
     <mergeCell ref="A31:G31"/>
@@ -2135,6 +2219,15 @@
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A22:G22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>